<commit_message>
add logging markers and log files by category
</commit_message>
<xml_diff>
--- a/src/test/resources/account.xlsx
+++ b/src/test/resources/account.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\christopher.g\eclipse-workspace\ecommerce.automation\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5FFF3B8-6174-4B8B-8579-32EC330460BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17DE83D7-2700-4AF6-86C4-15A8D8D63C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -670,7 +670,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>